<commit_message>
Created a loading screen that shows up the first time the app is loaded into memory. This is to give asyncstorage time to run all the loads that need to happen.
</commit_message>
<xml_diff>
--- a/Feature_Tracker.xlsx
+++ b/Feature_Tracker.xlsx
@@ -3,15 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72588593-838F-4CB1-82E2-62D611B3DF08}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99AA7F56-5192-4A22-B7E2-525F85CD44C9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$39</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$41</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
   <extLst>
@@ -718,24 +718,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="104.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="104.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -749,7 +748,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -766,7 +765,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -780,7 +779,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -794,7 +793,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -814,7 +813,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -831,7 +830,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -848,7 +847,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -862,7 +861,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -876,7 +875,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -890,7 +889,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -904,7 +903,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -918,7 +917,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -932,7 +931,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -946,7 +945,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -960,7 +959,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>49</v>
       </c>
@@ -977,7 +976,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>50</v>
       </c>
@@ -994,7 +993,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>53</v>
       </c>
@@ -1011,7 +1010,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>55</v>
       </c>
@@ -1025,7 +1024,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>57</v>
       </c>
@@ -1039,7 +1038,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>62</v>
       </c>
@@ -1053,7 +1052,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>66</v>
       </c>
@@ -1067,7 +1066,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>70</v>
       </c>
@@ -1081,7 +1080,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>72</v>
       </c>
@@ -1095,7 +1094,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>74</v>
       </c>
@@ -1109,7 +1108,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>78</v>
       </c>
@@ -1123,7 +1122,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>80</v>
       </c>
@@ -1137,7 +1136,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>84</v>
       </c>
@@ -1148,7 +1147,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>83</v>
       </c>
@@ -1159,7 +1158,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>85</v>
       </c>
@@ -1173,7 +1172,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>86</v>
       </c>
@@ -1184,7 +1183,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>87</v>
       </c>
@@ -1195,7 +1194,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>88</v>
       </c>
@@ -1209,7 +1208,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>89</v>
       </c>
@@ -1226,7 +1225,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>95</v>
       </c>
@@ -1240,7 +1239,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>105</v>
       </c>
@@ -1251,7 +1250,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>103</v>
       </c>
@@ -1265,7 +1264,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>107</v>
       </c>
@@ -1279,7 +1278,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>110</v>
       </c>
@@ -1290,7 +1289,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>119</v>
       </c>
@@ -1304,7 +1303,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>122</v>
       </c>
@@ -1319,11 +1318,8 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E39" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <filterColumn colId="2">
-      <filters blank="1"/>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:E41" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>